<commit_message>
data automation done, ready for start sending, also some .exe testing without success
</commit_message>
<xml_diff>
--- a/resources/peso-especifico.xlsx
+++ b/resources/peso-especifico.xlsx
@@ -77,7 +77,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -439,10 +439,10 @@
   <cols>
     <col min="1" max="1" style="5" width="16.005" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="6" width="24.14785714285714" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -453,7 +453,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -464,7 +464,7 @@
         <v>2.7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
@@ -475,7 +475,7 @@
         <v>7.81</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
@@ -486,7 +486,7 @@
         <v>7.81</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
@@ -497,7 +497,7 @@
         <v>7.9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="3" t="s">
         <v>11</v>
       </c>

</xml_diff>